<commit_message>
Add experiement sheet for results
</commit_message>
<xml_diff>
--- a/Arabic_Poetry_RNN/Experiement/Statistics.xlsx
+++ b/Arabic_Poetry_RNN/Experiement/Statistics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Experiment_Id</t>
   </si>
@@ -84,13 +84,49 @@
   </si>
   <si>
     <t>./Experiements_Logs/Experiment_Id_1_20171213022000.txt</t>
+  </si>
+  <si>
+    <t>validation</t>
+  </si>
+  <si>
+    <t>./Experiements_Logs/Experiment_Id_2_20171214022000.txt</t>
+  </si>
+  <si>
+    <t>First_Hidden_Layer_Units</t>
+  </si>
+  <si>
+    <t>Second_Hidden_Layer_Units</t>
+  </si>
+  <si>
+    <t>Forth_Hidden_Layer_Units</t>
+  </si>
+  <si>
+    <t>Third_Hidden_Layer_Units</t>
+  </si>
+  <si>
+    <t>./Experiements_Logs/Experiment_Id_3_20171216000000.txt</t>
+  </si>
+  <si>
+    <t>Fifth_Hidden_Layer_Units</t>
+  </si>
+  <si>
+    <t>Sixth_Hidden_Layer_Units</t>
+  </si>
+  <si>
+    <t>Dropout Per Layer</t>
+  </si>
+  <si>
+    <t>./Experiements_Logs/Experiment_Id_4_Z_20171216000000.txt</t>
+  </si>
+  <si>
+    <t>MISSED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +136,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -145,18 +188,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -468,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P15"/>
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -484,17 +531,19 @@
     <col min="6" max="6" width="8.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.46484375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.9296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="49.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="21.6640625" customWidth="1"/>
+    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="14.9296875" customWidth="1"/>
+    <col min="23" max="23" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="49.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -520,31 +569,55 @@
         <v>6</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="V1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -570,103 +643,345 @@
         <v>100</v>
       </c>
       <c r="I2" s="1">
+        <v>0</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+      <c r="M2" s="1">
+        <v>0</v>
+      </c>
+      <c r="N2" s="1">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1">
+        <v>0</v>
+      </c>
+      <c r="P2" s="1">
         <v>227615</v>
       </c>
-      <c r="J2" s="3">
+      <c r="Q2" s="3">
         <v>0.2</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="1">
-        <v>11</v>
-      </c>
-      <c r="N2" s="4">
+      <c r="T2" s="1">
+        <v>11</v>
+      </c>
+      <c r="U2" s="4">
         <v>0.91820000000000002</v>
       </c>
-      <c r="O2" s="4">
+      <c r="V2" s="4">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="W2" s="4">
         <v>0.91759999999999997</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.45">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="L6" s="1"/>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>20</v>
+      </c>
+      <c r="D3" s="1">
+        <v>64</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1">
+        <v>100</v>
+      </c>
+      <c r="I3" s="1">
+        <v>100</v>
+      </c>
+      <c r="J3" s="1">
+        <v>100</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+      <c r="M3" s="1">
+        <v>0</v>
+      </c>
+      <c r="N3" s="1">
+        <v>0</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0</v>
+      </c>
+      <c r="P3" s="1">
+        <v>227615</v>
+      </c>
+      <c r="Q3" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T3" s="1">
+        <v>11</v>
+      </c>
+      <c r="U3" s="4">
+        <v>0.96819999999999995</v>
+      </c>
+      <c r="V3" s="4">
+        <v>0.92900000000000005</v>
+      </c>
+      <c r="W3" s="4">
+        <v>0.93049999999999999</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>32</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1">
+        <v>3</v>
+      </c>
+      <c r="H4" s="1">
+        <v>500</v>
+      </c>
+      <c r="I4" s="1">
+        <v>500</v>
+      </c>
+      <c r="J4" s="1">
+        <v>500</v>
+      </c>
+      <c r="K4" s="1">
+        <v>500</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="1">
+        <v>0</v>
+      </c>
+      <c r="N4" s="1">
+        <v>0</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+      <c r="P4" s="1">
+        <v>227615</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T4" s="1">
+        <v>11</v>
+      </c>
+      <c r="U4" s="4">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="V4" s="4">
+        <v>0.95009999999999994</v>
+      </c>
+      <c r="W4" s="4">
+        <v>0.94820000000000004</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="H5" s="1">
+        <v>100</v>
+      </c>
+      <c r="I5" s="1">
+        <v>400</v>
+      </c>
+      <c r="J5" s="1">
+        <v>300</v>
+      </c>
+      <c r="K5" s="1">
+        <v>200</v>
+      </c>
+      <c r="L5" s="1">
+        <v>300</v>
+      </c>
+      <c r="M5" s="1">
+        <v>100</v>
+      </c>
+      <c r="N5" s="1">
+        <v>400</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="P5" s="1">
+        <v>227615</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T5" s="1">
+        <v>11</v>
+      </c>
+      <c r="U5" s="4">
+        <v>0.9375</v>
+      </c>
+      <c r="V5" s="4">
+        <v>0.88049999999999995</v>
+      </c>
+      <c r="W5" s="4">
+        <v>0.88080000000000003</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>500</v>
+      </c>
+      <c r="I6" s="1">
+        <v>500</v>
+      </c>
+      <c r="J6" s="1">
+        <v>500</v>
+      </c>
+      <c r="K6" s="1">
+        <v>500</v>
+      </c>
+      <c r="L6" s="1">
+        <v>500</v>
+      </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="P6" s="1">
+        <v>227615</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="R6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="T6" s="1">
+        <v>11</v>
+      </c>
+      <c r="U6" s="6">
+        <v>0.98770000000000002</v>
+      </c>
+      <c r="V6" s="5">
+        <v>95.21</v>
+      </c>
+      <c r="W6" s="5">
+        <v>93.21</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -683,8 +998,16 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -701,8 +1024,16 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -719,8 +1050,16 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -737,8 +1076,16 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -755,8 +1102,16 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -773,8 +1128,16 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -791,8 +1154,16 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -809,8 +1180,16 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.45">
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -827,6 +1206,14 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update experiement 6,7 results with logs
</commit_message>
<xml_diff>
--- a/Arabic_Poetry_RNN/Experiement/Statistics.xlsx
+++ b/Arabic_Poetry_RNN/Experiement/Statistics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="36">
   <si>
     <t>Experiment_Id</t>
   </si>
@@ -120,6 +120,18 @@
   </si>
   <si>
     <t>MISSED</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>3 LSTM 1 Dense 1 Dense Output</t>
+  </si>
+  <si>
+    <t>Experiment_Id_6.txt</t>
+  </si>
+  <si>
+    <t>3 LSTM with return sequence 1 Dense</t>
   </si>
 </sst>
 </file>
@@ -515,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X15"/>
+  <dimension ref="A1:Y15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Y8" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -530,20 +542,21 @@
     <col min="5" max="5" width="13.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.53125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="21.6640625" customWidth="1"/>
-    <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="14.9296875" customWidth="1"/>
-    <col min="23" max="23" width="14.265625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="49.265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.73046875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="21.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="14.9296875" customWidth="1"/>
+    <col min="24" max="24" width="14.265625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="49.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -566,58 +579,61 @@
         <v>5</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -639,12 +655,10 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1">
         <v>100</v>
       </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
       <c r="J2" s="1">
         <v>0</v>
       </c>
@@ -664,34 +678,37 @@
         <v>0</v>
       </c>
       <c r="P2" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="1">
         <v>227615</v>
       </c>
-      <c r="Q2" s="3">
+      <c r="R2" s="3">
         <v>0.2</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T2" s="1">
-        <v>11</v>
-      </c>
-      <c r="U2" s="4">
+      <c r="U2" s="1">
+        <v>11</v>
+      </c>
+      <c r="V2" s="4">
         <v>0.91820000000000002</v>
       </c>
-      <c r="V2" s="4">
+      <c r="W2" s="4">
         <v>0.92500000000000004</v>
       </c>
-      <c r="W2" s="4">
+      <c r="X2" s="4">
         <v>0.91759999999999997</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -713,9 +730,7 @@
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
-        <v>100</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1">
         <v>100</v>
       </c>
@@ -723,7 +738,7 @@
         <v>100</v>
       </c>
       <c r="K3" s="1">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="L3" s="1">
         <v>0</v>
@@ -738,34 +753,37 @@
         <v>0</v>
       </c>
       <c r="P3" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="1">
         <v>227615</v>
       </c>
-      <c r="Q3" s="3">
+      <c r="R3" s="3">
         <v>0.2</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="1" t="s">
+      <c r="T3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T3" s="1">
-        <v>11</v>
-      </c>
-      <c r="U3" s="4">
+      <c r="U3" s="1">
+        <v>11</v>
+      </c>
+      <c r="V3" s="4">
         <v>0.96819999999999995</v>
       </c>
-      <c r="V3" s="4">
+      <c r="W3" s="4">
         <v>0.92900000000000005</v>
       </c>
-      <c r="W3" s="4">
+      <c r="X3" s="4">
         <v>0.93049999999999999</v>
       </c>
-      <c r="X3" s="1" t="s">
+      <c r="Y3" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -787,9 +805,7 @@
       <c r="G4" s="1">
         <v>3</v>
       </c>
-      <c r="H4" s="1">
-        <v>500</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1">
         <v>500</v>
       </c>
@@ -800,7 +816,7 @@
         <v>500</v>
       </c>
       <c r="L4" s="1">
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="M4" s="1">
         <v>0</v>
@@ -812,34 +828,37 @@
         <v>0</v>
       </c>
       <c r="P4" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="1">
         <v>227615</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="3">
         <v>0.2</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="1" t="s">
+      <c r="T4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T4" s="1">
-        <v>11</v>
-      </c>
-      <c r="U4" s="4">
+      <c r="U4" s="1">
+        <v>11</v>
+      </c>
+      <c r="V4" s="4">
         <v>0.98899999999999999</v>
       </c>
-      <c r="V4" s="4">
+      <c r="W4" s="4">
         <v>0.95009999999999994</v>
       </c>
-      <c r="W4" s="4">
+      <c r="X4" s="4">
         <v>0.94820000000000004</v>
       </c>
-      <c r="X4" s="1" t="s">
+      <c r="Y4" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -861,59 +880,60 @@
       <c r="G5" s="1">
         <v>6</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
         <v>100</v>
       </c>
-      <c r="I5" s="1">
+      <c r="J5" s="1">
         <v>400</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <v>300</v>
       </c>
-      <c r="K5" s="1">
+      <c r="L5" s="1">
         <v>200</v>
       </c>
-      <c r="L5" s="1">
+      <c r="M5" s="1">
         <v>300</v>
       </c>
-      <c r="M5" s="1">
+      <c r="N5" s="1">
         <v>100</v>
       </c>
-      <c r="N5" s="1">
+      <c r="O5" s="1">
         <v>400</v>
       </c>
-      <c r="O5" s="1">
+      <c r="P5" s="1">
         <v>0.1</v>
       </c>
-      <c r="P5" s="1">
+      <c r="Q5" s="1">
         <v>227615</v>
       </c>
-      <c r="Q5" s="3">
+      <c r="R5" s="3">
         <v>0.2</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T5" s="1">
-        <v>11</v>
-      </c>
-      <c r="U5" s="4">
+      <c r="U5" s="1">
+        <v>11</v>
+      </c>
+      <c r="V5" s="4">
         <v>0.9375</v>
       </c>
-      <c r="V5" s="4">
+      <c r="W5" s="4">
         <v>0.88049999999999995</v>
       </c>
-      <c r="W5" s="4">
+      <c r="X5" s="4">
         <v>0.88080000000000003</v>
       </c>
-      <c r="X5" s="1" t="s">
+      <c r="Y5" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -935,9 +955,7 @@
       <c r="G6" s="1">
         <v>4</v>
       </c>
-      <c r="H6" s="1">
-        <v>500</v>
-      </c>
+      <c r="H6" s="1"/>
       <c r="I6" s="1">
         <v>500</v>
       </c>
@@ -950,90 +968,179 @@
       <c r="L6" s="1">
         <v>500</v>
       </c>
-      <c r="M6" s="1"/>
+      <c r="M6" s="1">
+        <v>500</v>
+      </c>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="1">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1">
         <v>227615</v>
       </c>
-      <c r="Q6" s="3">
+      <c r="R6" s="3">
         <v>0.2</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S6" s="1" t="s">
+      <c r="T6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T6" s="1">
-        <v>11</v>
-      </c>
-      <c r="U6" s="6">
+      <c r="U6" s="1">
+        <v>11</v>
+      </c>
+      <c r="V6" s="6">
         <v>0.98770000000000002</v>
       </c>
-      <c r="V6" s="5">
+      <c r="W6" s="5">
         <v>95.21</v>
       </c>
-      <c r="W6" s="5">
+      <c r="X6" s="5">
         <v>93.21</v>
       </c>
-      <c r="X6" s="1" t="s">
+      <c r="Y6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1">
+        <v>50</v>
+      </c>
+      <c r="D7" s="1">
+        <v>50</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="1">
+        <v>5</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I7" s="1">
+        <v>300</v>
+      </c>
+      <c r="J7" s="1">
+        <v>300</v>
+      </c>
+      <c r="K7" s="1">
+        <v>300</v>
+      </c>
+      <c r="L7" s="1">
+        <v>300</v>
+      </c>
+      <c r="M7" s="1">
+        <v>300</v>
+      </c>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-      <c r="Q7" s="1"/>
-      <c r="R7" s="1"/>
-      <c r="S7" s="1"/>
-      <c r="T7" s="1"/>
-      <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="1"/>
-      <c r="X7" s="1"/>
-    </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
+      <c r="Q7" s="1">
+        <v>227615</v>
+      </c>
+      <c r="R7" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="S7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U7" s="1">
+        <v>11</v>
+      </c>
+      <c r="V7" s="6">
+        <v>0.98899999999999999</v>
+      </c>
+      <c r="W7" s="6">
+        <v>0.94020000000000004</v>
+      </c>
+      <c r="X7" s="4">
+        <v>0.94079999999999997</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>11</v>
+      </c>
+      <c r="C8" s="1">
+        <v>20</v>
+      </c>
+      <c r="D8" s="1">
+        <v>50</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="1">
+        <v>1000</v>
+      </c>
+      <c r="K8" s="1">
+        <v>1000</v>
+      </c>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
-      <c r="Q8" s="1"/>
-      <c r="R8" s="1"/>
-      <c r="S8" s="1"/>
-      <c r="T8" s="1"/>
-      <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="1"/>
-      <c r="X8" s="1"/>
-    </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="P8" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="Q8" s="1">
+        <v>227615</v>
+      </c>
+      <c r="R8" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U8" s="1">
+        <v>11</v>
+      </c>
+      <c r="V8" s="6">
+        <v>0.9879</v>
+      </c>
+      <c r="W8" s="4">
+        <v>0.96350000000000002</v>
+      </c>
+      <c r="X8" s="4">
+        <v>0.96709999999999996</v>
+      </c>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1058,8 +1165,9 @@
       <c r="V9" s="1"/>
       <c r="W9" s="1"/>
       <c r="X9" s="1"/>
-    </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y9" s="1"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1084,8 +1192,9 @@
       <c r="V10" s="1"/>
       <c r="W10" s="1"/>
       <c r="X10" s="1"/>
-    </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -1110,8 +1219,9 @@
       <c r="V11" s="1"/>
       <c r="W11" s="1"/>
       <c r="X11" s="1"/>
-    </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y11" s="1"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1136,8 +1246,9 @@
       <c r="V12" s="1"/>
       <c r="W12" s="1"/>
       <c r="X12" s="1"/>
-    </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1162,8 +1273,9 @@
       <c r="V13" s="1"/>
       <c r="W13" s="1"/>
       <c r="X13" s="1"/>
-    </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y13" s="1"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1188,8 +1300,9 @@
       <c r="V14" s="1"/>
       <c r="W14" s="1"/>
       <c r="X14" s="1"/>
-    </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="Y14" s="1"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.45">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1214,6 +1327,7 @@
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
       <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>